<commit_message>
Created plots and updated exel
</commit_message>
<xml_diff>
--- a/results/iceBook.xlsx
+++ b/results/iceBook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suren Gourapura\Documents\OSU\Research\SurenRepo\iceberg\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suren Gourapura\Documents\OSU\Research\Iceberg\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="7">
-  <si>
-    <t>Denoising</t>
-  </si>
-  <si>
-    <t>Trimsize</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
   <si>
     <t>train</t>
   </si>
@@ -38,13 +32,58 @@
     <t>test</t>
   </si>
   <si>
-    <t>Train/Test</t>
+    <t>Accuracy1</t>
   </si>
   <si>
-    <t>Including</t>
+    <t>Train/Test1</t>
   </si>
   <si>
-    <t>Accuracy</t>
+    <t>Train/Test2</t>
+  </si>
+  <si>
+    <t>Denoising1</t>
+  </si>
+  <si>
+    <t>Trimsize1</t>
+  </si>
+  <si>
+    <t>Including2</t>
+  </si>
+  <si>
+    <t>Denoising3</t>
+  </si>
+  <si>
+    <t>avgAcc3</t>
+  </si>
+  <si>
+    <t>2trial1</t>
+  </si>
+  <si>
+    <t>3trial1</t>
+  </si>
+  <si>
+    <t>3trial2</t>
+  </si>
+  <si>
+    <t>3trial3</t>
+  </si>
+  <si>
+    <t>incl4</t>
+  </si>
+  <si>
+    <t>4trial1</t>
+  </si>
+  <si>
+    <t>4trial2</t>
+  </si>
+  <si>
+    <t>avgAcc4</t>
+  </si>
+  <si>
+    <t>stDev3</t>
+  </si>
+  <si>
+    <t>stDev4</t>
   </si>
 </sst>
 </file>
@@ -97,6 +136,3229 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pseudo-Label</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Data Augmentation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$N$2:$N$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.149999999999987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.099999999999997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.099999999999997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.4500000000000122E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.149999999999987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.7500000000000329E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$N$2:$N$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.149999999999987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.099999999999997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.099999999999997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.4500000000000122E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.149999999999987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.7500000000000329E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$N$2:$N$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.149999999999987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.099999999999997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.099999999999997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.4500000000000122E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.149999999999987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.7500000000000329E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$N$2:$N$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.149999999999987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.099999999999997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.099999999999997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.4500000000000122E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.149999999999987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.7500000000000329E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90644999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89980000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90975000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91305000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90315000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9CF7-497C-9879-329FBD312B0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>trial1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8891</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89070000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89739999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9CF7-497C-9879-329FBD312B0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>trial2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91059999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9073</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91720000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91720000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9CF7-497C-9879-329FBD312B0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="431164992"/>
+        <c:axId val="431164336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="431164992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Inculded amount</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Testing Data with Pseudo-Labels</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="431164336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="431164336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.92"/>
+          <c:min val="0.88000000000000012"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="431164992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Denoising</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3trial1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.88249999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87090000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90559999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90559999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.91559999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91059999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.90229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.89739999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9073</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.90069999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-018C-48E3-981A-B0D1F9FA9371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3trial2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.91390000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91059999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90559999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90559999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90559999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90559999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9073</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.90559999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9073</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.90069999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.90559999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-018C-48E3-981A-B0D1F9FA9371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3trial3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$U$2:$U$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>1.6110452093801346E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.8327211098982478E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.0401524997465939E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5424723326562003E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.1584102892999307E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1112698372207804E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.0824829046386341E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.3688289811649357E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.0960825307915844E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.3880441875771174E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1112698372208333E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.1288147682486832E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>8.5000000000001741E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$U$2:$U$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>1.6110452093801346E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.8327211098982478E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.0401524997465939E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5424723326562003E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.1584102892999307E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1112698372207804E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.0824829046386341E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.3688289811649357E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.0960825307915844E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.3880441875771174E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1112698372208333E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.1288147682486832E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>8.5000000000001741E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.91890000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9123</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9123</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9073</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91390000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9123</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.90890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.91390000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-018C-48E3-981A-B0D1F9FA9371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>avgAcc3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$U$2:$U$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>1.6110452093801346E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.8327211098982478E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.0401524997465939E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5424723326562003E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.1584102892999307E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1112698372207804E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.0824829046386341E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.3688289811649357E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.0960825307915844E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.3880441875771174E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1112698372208333E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.1288147682486832E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>8.5000000000001741E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$U$2:$U$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>1.6110452093801346E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.8327211098982478E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.0401524997465939E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5424723326562003E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.1584102892999307E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1112698372207804E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.0824829046386341E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.3688289811649357E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.0960825307915844E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.3880441875771174E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1112698372208333E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.1288147682486832E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>8.5000000000001741E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$2:$T$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.90510000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89679999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90616666666666668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90506666666666657</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90783333333333338</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90119999999999989</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90730000000000011</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.90949999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90673333333333339</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91060000000000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.90669999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.90399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.90644999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.90069999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-018C-48E3-981A-B0D1F9FA9371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="345524656"/>
+        <c:axId val="345537448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="345524656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Denoising Strength (h)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="345537448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="345537448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="345524656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>408389</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>77694</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>488078</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>15687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D19FD7A3-7031-4D8F-9D46-D155A473100D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>191744</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>239060</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>139451</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4543F62-1185-4D5E-A7EC-3D67BDD0B59D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,41 +3658,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="13" max="13" width="9.46875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -441,7 +3737,7 @@
         <v>0.89980000000000004</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -450,10 +3746,47 @@
         <v>0.90200000000000002</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="L2">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="M2">
+        <f>AVERAGE(K2:L2)</f>
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="N2">
+        <f>_xlfn.STDEV.P(K2:L2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="R2">
+        <v>0.91390000000000005</v>
+      </c>
+      <c r="S2">
+        <v>0.91890000000000005</v>
+      </c>
+      <c r="T2">
+        <f>AVERAGE(Q2:S2)</f>
+        <v>0.90510000000000002</v>
+      </c>
+      <c r="U2">
+        <f>_xlfn.STDEV.P(Q2:S2)</f>
+        <v>1.6110452093801346E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>0</v>
       </c>
@@ -464,7 +3797,7 @@
         <v>0.93969999999999998</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -473,10 +3806,47 @@
         <v>0.90229999999999999</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>250</v>
+      </c>
+      <c r="K3">
+        <v>0.90229999999999999</v>
+      </c>
+      <c r="L3">
+        <v>0.91059999999999997</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M8" si="0">AVERAGE(K3:L3)</f>
+        <v>0.90644999999999998</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N8" si="1">_xlfn.STDEV.P(K3:L3)</f>
+        <v>4.149999999999987E-3</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>0.87090000000000001</v>
+      </c>
+      <c r="R3">
+        <v>0.91059999999999997</v>
+      </c>
+      <c r="S3">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T13" si="2">AVERAGE(Q3:S3)</f>
+        <v>0.89679999999999993</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U15" si="3">_xlfn.STDEV.P(Q3:S3)</f>
+        <v>1.8327211098982478E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>5</v>
       </c>
@@ -487,7 +3857,7 @@
         <v>0.93400000000000005</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>250</v>
@@ -496,10 +3866,47 @@
         <v>0.76719999999999999</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>500</v>
+      </c>
+      <c r="K4">
+        <v>0.8891</v>
+      </c>
+      <c r="L4">
+        <v>0.9073</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0.8982</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>9.099999999999997E-3</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="R4">
+        <v>0.90559999999999996</v>
+      </c>
+      <c r="S4">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="2"/>
+        <v>0.90616666666666668</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="3"/>
+        <v>2.0401524997465939E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>5</v>
       </c>
@@ -510,7 +3917,7 @@
         <v>0.94950000000000001</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>250</v>
@@ -519,10 +3926,47 @@
         <v>0.90229999999999999</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1000</v>
+      </c>
+      <c r="K5">
+        <v>0.89070000000000005</v>
+      </c>
+      <c r="L5">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.89980000000000004</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>9.099999999999997E-3</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>0.90559999999999996</v>
+      </c>
+      <c r="R5">
+        <v>0.90559999999999996</v>
+      </c>
+      <c r="S5">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="2"/>
+        <v>0.90506666666666657</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="3"/>
+        <v>7.5424723326562003E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -533,7 +3977,7 @@
         <v>0.95120000000000005</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>500</v>
@@ -542,10 +3986,47 @@
         <v>0.61670000000000003</v>
       </c>
       <c r="H6" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>2000</v>
+      </c>
+      <c r="K6">
+        <v>0.90229999999999999</v>
+      </c>
+      <c r="L6">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.90975000000000006</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>7.4500000000000122E-3</v>
+      </c>
+      <c r="P6">
+        <v>12</v>
+      </c>
+      <c r="Q6">
+        <v>0.90559999999999996</v>
+      </c>
+      <c r="R6">
+        <v>0.90559999999999996</v>
+      </c>
+      <c r="S6">
+        <v>0.9123</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>0.90783333333333338</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="3"/>
+        <v>3.1584102892999307E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>10</v>
       </c>
@@ -556,7 +4037,7 @@
         <v>0.90200000000000002</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>500</v>
@@ -565,10 +4046,47 @@
         <v>0.8891</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>4000</v>
+      </c>
+      <c r="K7">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="L7">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0.91305000000000003</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>4.149999999999987E-3</v>
+      </c>
+      <c r="P7">
+        <v>13</v>
+      </c>
+      <c r="Q7">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="R7">
+        <v>0.90559999999999996</v>
+      </c>
+      <c r="S7">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>0.90119999999999989</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="3"/>
+        <v>3.1112698372207804E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>10</v>
       </c>
@@ -579,7 +4097,7 @@
         <v>0.96960000000000002</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>1000</v>
@@ -588,10 +4106,47 @@
         <v>0.47</v>
       </c>
       <c r="H8" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>8000</v>
+      </c>
+      <c r="K8">
+        <v>0.89739999999999998</v>
+      </c>
+      <c r="L8">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.90315000000000001</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>5.7500000000000329E-3</v>
+      </c>
+      <c r="P8">
+        <v>14</v>
+      </c>
+      <c r="Q8">
+        <v>0.90229999999999999</v>
+      </c>
+      <c r="R8">
+        <v>0.9073</v>
+      </c>
+      <c r="S8">
+        <v>0.9123</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>0.90730000000000011</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="3"/>
+        <v>4.0824829046386341E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>10</v>
       </c>
@@ -602,7 +4157,7 @@
         <v>0.95299999999999996</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>1000</v>
@@ -611,10 +4166,30 @@
         <v>0.89070000000000005</v>
       </c>
       <c r="H9" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>15</v>
+      </c>
+      <c r="Q9">
+        <v>0.91559999999999997</v>
+      </c>
+      <c r="R9">
+        <v>0.90559999999999996</v>
+      </c>
+      <c r="S9">
+        <v>0.9073</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>0.90949999999999998</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="3"/>
+        <v>4.3688289811649357E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>0</v>
       </c>
@@ -625,7 +4200,7 @@
         <v>0.87909999999999999</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>2000</v>
@@ -634,10 +4209,30 @@
         <v>0.32700000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>16</v>
+      </c>
+      <c r="Q10">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="R10">
+        <v>0.9073</v>
+      </c>
+      <c r="S10">
+        <v>0.91390000000000005</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>0.90673333333333339</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="3"/>
+        <v>6.0960825307915844E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>0</v>
       </c>
@@ -648,7 +4243,7 @@
         <v>0.87909999999999999</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>2000</v>
@@ -657,10 +4252,30 @@
         <v>0.90229999999999999</v>
       </c>
       <c r="H11" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>17</v>
+      </c>
+      <c r="Q11">
+        <v>0.91059999999999997</v>
+      </c>
+      <c r="R11">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="S11">
+        <v>0.9123</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>0.91060000000000008</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="3"/>
+        <v>1.3880441875771174E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>5</v>
       </c>
@@ -671,7 +4286,7 @@
         <v>0.87090000000000001</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>4000</v>
@@ -680,10 +4295,30 @@
         <v>0.1986</v>
       </c>
       <c r="H12" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>18</v>
+      </c>
+      <c r="Q12">
+        <v>0.90229999999999999</v>
+      </c>
+      <c r="R12">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="S12">
+        <v>0.90890000000000004</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>0.90669999999999995</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="3"/>
+        <v>3.1112698372208333E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>5</v>
       </c>
@@ -694,7 +4329,7 @@
         <v>0.88080000000000003</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>4000</v>
@@ -703,10 +4338,30 @@
         <v>0.90890000000000004</v>
       </c>
       <c r="H13" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>20</v>
+      </c>
+      <c r="Q13">
+        <v>0.89739999999999998</v>
+      </c>
+      <c r="R13">
+        <v>0.90069999999999995</v>
+      </c>
+      <c r="S13">
+        <v>0.91390000000000005</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>0.90399999999999991</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="3"/>
+        <v>7.1288147682486832E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>5</v>
       </c>
@@ -717,7 +4372,7 @@
         <v>0.87749999999999995</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>8000</v>
@@ -726,10 +4381,27 @@
         <v>0.1149</v>
       </c>
       <c r="H14" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>25</v>
+      </c>
+      <c r="Q14">
+        <v>0.9073</v>
+      </c>
+      <c r="R14">
+        <v>0.90559999999999996</v>
+      </c>
+      <c r="T14">
+        <f>AVERAGE(Q14:R14)</f>
+        <v>0.90644999999999998</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="3"/>
+        <v>8.5000000000001741E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>10</v>
       </c>
@@ -740,7 +4412,7 @@
         <v>0.90229999999999999</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>8000</v>
@@ -749,10 +4421,24 @@
         <v>0.89739999999999998</v>
       </c>
       <c r="H15" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>30</v>
+      </c>
+      <c r="Q15">
+        <v>0.90069999999999995</v>
+      </c>
+      <c r="T15">
+        <f>Q15</f>
+        <v>0.90069999999999995</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>10</v>
       </c>
@@ -763,7 +4449,7 @@
         <v>0.89739999999999998</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
@@ -777,7 +4463,7 @@
         <v>0.8841</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
@@ -791,7 +4477,7 @@
         <v>0.93300000000000005</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
@@ -805,7 +4491,7 @@
         <v>0.88249999999999995</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
@@ -819,7 +4505,7 @@
         <v>0.93149999999999999</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
@@ -833,7 +4519,7 @@
         <v>0.91559999999999997</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.5">
@@ -847,7 +4533,7 @@
         <v>0.96160000000000001</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.5">
@@ -861,7 +4547,7 @@
         <v>0.8891</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.5">
@@ -875,7 +4561,7 @@
         <v>0.94879999999999998</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.5">
@@ -889,7 +4575,7 @@
         <v>0.8841</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.5">
@@ -903,7 +4589,7 @@
         <v>0.9325</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.5">
@@ -917,7 +4603,7 @@
         <v>0.89739999999999998</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.5">
@@ -931,7 +4617,7 @@
         <v>0.9667</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.5">
@@ -945,7 +4631,7 @@
         <v>0.88080000000000003</v>
       </c>
       <c r="D29" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
@@ -959,7 +4645,7 @@
         <v>0.94920000000000004</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
@@ -973,7 +4659,7 @@
         <v>0.8659</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
@@ -987,7 +4673,7 @@
         <v>0.98299999999999998</v>
       </c>
       <c r="D32" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.5">
@@ -1001,7 +4687,7 @@
         <v>0.98099999999999998</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.5">
@@ -1015,7 +4701,7 @@
         <v>0.97350000000000003</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.5">
@@ -1029,7 +4715,7 @@
         <v>0.97150000000000003</v>
       </c>
       <c r="D35" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.5">
@@ -1043,7 +4729,7 @@
         <v>0.97850000000000004</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.5">
@@ -1057,7 +4743,7 @@
         <v>0.96799999999999997</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.5">
@@ -1071,7 +4757,7 @@
         <v>0.97299999999999998</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.5">
@@ -1085,7 +4771,7 @@
         <v>0.90559999999999996</v>
       </c>
       <c r="D39" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.5">
@@ -1099,7 +4785,7 @@
         <v>0.90559999999999996</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.5">
@@ -1113,7 +4799,7 @@
         <v>0.89900000000000002</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.5">
@@ -1127,7 +4813,7 @@
         <v>0.90229999999999999</v>
       </c>
       <c r="D42" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.5">
@@ -1141,7 +4827,7 @@
         <v>0.89900000000000002</v>
       </c>
       <c r="D43" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.5">
@@ -1155,7 +4841,7 @@
         <v>0.91059999999999997</v>
       </c>
       <c r="D44" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.5">
@@ -1169,10 +4855,11 @@
         <v>0.90229999999999999</v>
       </c>
       <c r="D45" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>